<commit_message>
Corrige estrutura de Resources
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-BRTurno.xlsx
+++ b/docs/StructureDefinition-BRTurno.xlsx
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Turno do Dia</t>
+    <t>Turno</t>
   </si>
   <si>
     <t>Status</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-21T18:35:12-03:00</t>
+    <t>2024-02-07T09:19:37-03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>